<commit_message>
Fixed display, added data
</commit_message>
<xml_diff>
--- a/output/dnc__runtime.xlsx
+++ b/output/dnc__runtime.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,11 +446,245 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.00043320655822753906   1478.7844496356363</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.0013828277587890625   1586.6035551964073</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.0011568069458007812   2700.169578241978</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.0011398792266845703   2304.1943061377356</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.0010950565338134766   2170.1550130241067</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.00152587890625   3115.612463503049</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.0016062259674072266   3125.1921031396837</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.001445770263671875   3489.6052035718785</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
         <v>11</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.0008068084716796875   3623.536093755979</t>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.0016651153564453125   3144.306360735204</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.0015218257904052734   2615.772701031637</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>13</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.0019140243530273438   3606.5551405276406</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>14</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.0014998912811279297   3416.7253329298414</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.0018990039825439453   4020.474060169532</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.0018758773803710938   3584.757340944614</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>32</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.003821134567260742   6191.340337976364</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>64</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.009843826293945312   7599.793185869602</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>128</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.034120798110961914   10419.950572657754</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>256</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.08082199096679688   14476.415242859599</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>512</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.2781088352203369   20928.834848824987</t>
         </is>
       </c>
     </row>

</xml_diff>